<commit_message>
TAC-3111, Fix save vases from import dto, Fix origin facility in import trip, Add some enhancements in import trip
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportShipmentSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportShipmentSampleFile.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25122"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF952177-6F03-4FB3-ADA7-BD3C8688CF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E459C66-6F13-448B-A1A9-3E8DBE0D101F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Reference No</t>
   </si>
@@ -49,7 +50,10 @@
     <t>Has Attchment ?*</t>
   </si>
   <si>
-    <t>10/21/2021</t>
+    <t>Original Facility*</t>
+  </si>
+  <si>
+    <t>Destination Facility*</t>
   </si>
   <si>
     <t>nooooooootes</t>
@@ -61,10 +65,10 @@
     <t>no</t>
   </si>
   <si>
-    <t>10/22/2021</t>
-  </si>
-  <si>
-    <t>llklk</t>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test12</t>
   </si>
 </sst>
 </file>
@@ -417,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -431,10 +435,11 @@
     <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,48 +461,43 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44639</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2">
         <v>1120</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
+    <row r="3" spans="1:9">
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3">
-        <v>120</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
TAC-3104, Fix start trip date issue
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportShipmentSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportShipmentSampleFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25122"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1827F6FB-3E46-41F9-A655-6415F6743364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D24A5C49-0739-402E-BBC8-6E814778C1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Reference No</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Destination Facility*</t>
+  </si>
+  <si>
+    <t>03/19/2022</t>
   </si>
   <si>
     <t>nooooooootes</t>
@@ -75,6 +78,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-1010000]m/d/yyyy;@"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -104,9 +110,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +431,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -470,29 +477,29 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44639</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2">
         <v>1120</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9">

</xml_diff>

<commit_message>
TAC-3702  Fix validate date format in excel
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportShipmentSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportShipmentSampleFile.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D24A5C49-0739-402E-BBC8-6E814778C1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tachyon_13062022\tachyon-core\angular\src\assets\sampleFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2919FDD8-1394-4357-863E-7BE176DC466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,9 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -32,12 +35,6 @@
     <t>Reference No</t>
   </si>
   <si>
-    <t>Trip Pick up Date Start *</t>
-  </si>
-  <si>
-    <t>Trip Pick up Date End</t>
-  </si>
-  <si>
     <t>Approximate Total Value of Goods</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Destination Facility*</t>
   </si>
   <si>
-    <t>03/19/2022</t>
-  </si>
-  <si>
     <t>nooooooootes</t>
   </si>
   <si>
@@ -68,20 +62,26 @@
     <t>no</t>
   </si>
   <si>
-    <t>test11</t>
-  </si>
-  <si>
-    <t>test12</t>
+    <t>Trip Pick up Date Start MM/dd/YYYY (Text Format) *</t>
+  </si>
+  <si>
+    <t>Trip Pick up Date End  MM/dd/YYYY (Text Format) *</t>
+  </si>
+  <si>
+    <t>2022/06/29</t>
+  </si>
+  <si>
+    <t>pickup 3</t>
+  </si>
+  <si>
+    <t>drop 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-1010000]m/d/yyyy;@"/>
-  </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,7 +113,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,69 +431,69 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2">
         <v>1120</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -502,8 +502,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="B3" s="1"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
       <c r="C3" s="1"/>
     </row>
   </sheetData>
@@ -513,5 +513,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>